<commit_message>
Update Excel simple test cases
</commit_message>
<xml_diff>
--- a/reeevr/test/excelunit/simple-tests.xlsx
+++ b/reeevr/test/excelunit/simple-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mo14776\PycharmProjects\Excel-R-compiler\reeevr\test\excelunit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EBFDF2-E824-4034-9994-80079A292E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5719D-4BE8-4A93-BFCA-747E861A3B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AEC3FC54-0D47-4937-A0CF-B72916A7CC33}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="B2:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>